<commit_message>
Updated tests for running mean temp and max adaptive
</commit_message>
<xml_diff>
--- a/tests/testdata/tm52/TM52__TestJob1.xlsx
+++ b/tests/testdata/tm52/TM52__TestJob1.xlsx
@@ -27,18 +27,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="133">
   <si>
+    <t>JobNo</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>JobNo</t>
-  </si>
-  <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -72,12 +72,12 @@
     <t>10</t>
   </si>
   <si>
-    <t>20220222</t>
-  </si>
-  <si>
     <t>/c/e</t>
   </si>
   <si>
+    <t>jovyan</t>
+  </si>
+  <si>
     <t>Project Information</t>
   </si>
   <si>
@@ -111,7 +111,7 @@
     <t>Results, Air Speed 0.8</t>
   </si>
   <si>
-    <t>jovyan</t>
+    <t>20220223</t>
   </si>
   <si>
     <t>index</t>
@@ -180,7 +180,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-02-22 19:34:54.790065</t>
+    <t>2022-02-23 16:02:16.314492</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -607,10 +607,10 @@
   <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="Date"/>
-    <tableColumn id="3" name="JobNo"/>
+    <tableColumn id="2" name="JobNo"/>
+    <tableColumn id="3" name="Author"/>
     <tableColumn id="4" name="sheet_name"/>
-    <tableColumn id="5" name="Author"/>
+    <tableColumn id="5" name="Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4683,7 +4683,7 @@
         <v>100</v>
       </c>
       <c r="D2">
-        <v>2.48</v>
+        <v>2.5</v>
       </c>
       <c r="E2" t="s">
         <v>131</v>
@@ -4715,7 +4715,7 @@
         <v>101</v>
       </c>
       <c r="D3">
-        <v>7.89</v>
+        <v>7.9</v>
       </c>
       <c r="E3" t="s">
         <v>132</v>
@@ -4747,7 +4747,7 @@
         <v>102</v>
       </c>
       <c r="D4">
-        <v>8.039999999999999</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
         <v>132</v>
@@ -4907,7 +4907,7 @@
         <v>107</v>
       </c>
       <c r="D9">
-        <v>10.59</v>
+        <v>10.6</v>
       </c>
       <c r="E9" t="s">
         <v>132</v>
@@ -4939,7 +4939,7 @@
         <v>108</v>
       </c>
       <c r="D10">
-        <v>26.04</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
         <v>132</v>
@@ -4971,7 +4971,7 @@
         <v>109</v>
       </c>
       <c r="D11">
-        <v>11.57</v>
+        <v>11.6</v>
       </c>
       <c r="E11" t="s">
         <v>132</v>
@@ -5099,7 +5099,7 @@
         <v>113</v>
       </c>
       <c r="D15">
-        <v>0.14</v>
+        <v>0.1</v>
       </c>
       <c r="E15" t="s">
         <v>131</v>
@@ -5163,7 +5163,7 @@
         <v>115</v>
       </c>
       <c r="D17">
-        <v>12.94</v>
+        <v>12.9</v>
       </c>
       <c r="E17" t="s">
         <v>132</v>
@@ -5195,7 +5195,7 @@
         <v>116</v>
       </c>
       <c r="D18">
-        <v>28.26</v>
+        <v>28.3</v>
       </c>
       <c r="E18" t="s">
         <v>132</v>
@@ -5227,7 +5227,7 @@
         <v>117</v>
       </c>
       <c r="D19">
-        <v>13.45</v>
+        <v>13.5</v>
       </c>
       <c r="E19" t="s">
         <v>132</v>
@@ -5259,7 +5259,7 @@
         <v>118</v>
       </c>
       <c r="D20">
-        <v>28.46</v>
+        <v>28.5</v>
       </c>
       <c r="E20" t="s">
         <v>132</v>
@@ -5291,7 +5291,7 @@
         <v>119</v>
       </c>
       <c r="D21">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="E21" t="s">
         <v>131</v>
@@ -5323,7 +5323,7 @@
         <v>120</v>
       </c>
       <c r="D22">
-        <v>1.58</v>
+        <v>1.6</v>
       </c>
       <c r="E22" t="s">
         <v>131</v>
@@ -5355,7 +5355,7 @@
         <v>121</v>
       </c>
       <c r="D23">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="E23" t="s">
         <v>131</v>
@@ -5387,7 +5387,7 @@
         <v>122</v>
       </c>
       <c r="D24">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="E24" t="s">
         <v>131</v>
@@ -5419,7 +5419,7 @@
         <v>123</v>
       </c>
       <c r="D25">
-        <v>5.61</v>
+        <v>5.6</v>
       </c>
       <c r="E25" t="s">
         <v>132</v>
@@ -5483,7 +5483,7 @@
         <v>125</v>
       </c>
       <c r="D27">
-        <v>5.23</v>
+        <v>5.2</v>
       </c>
       <c r="E27" t="s">
         <v>132</v>
@@ -5515,7 +5515,7 @@
         <v>126</v>
       </c>
       <c r="D28">
-        <v>17.75</v>
+        <v>17.7</v>
       </c>
       <c r="E28" t="s">
         <v>132</v>
@@ -5728,7 +5728,7 @@
         <v>100</v>
       </c>
       <c r="D2">
-        <v>0.63</v>
+        <v>0.6</v>
       </c>
       <c r="E2" t="s">
         <v>131</v>
@@ -5760,7 +5760,7 @@
         <v>101</v>
       </c>
       <c r="D3">
-        <v>1.71</v>
+        <v>1.7</v>
       </c>
       <c r="E3" t="s">
         <v>131</v>
@@ -5792,7 +5792,7 @@
         <v>102</v>
       </c>
       <c r="D4">
-        <v>1.76</v>
+        <v>1.8</v>
       </c>
       <c r="E4" t="s">
         <v>131</v>
@@ -5952,7 +5952,7 @@
         <v>107</v>
       </c>
       <c r="D9">
-        <v>4.19</v>
+        <v>4.2</v>
       </c>
       <c r="E9" t="s">
         <v>132</v>
@@ -5984,7 +5984,7 @@
         <v>108</v>
       </c>
       <c r="D10">
-        <v>12.57</v>
+        <v>12.6</v>
       </c>
       <c r="E10" t="s">
         <v>132</v>
@@ -6016,7 +6016,7 @@
         <v>109</v>
       </c>
       <c r="D11">
-        <v>3.92</v>
+        <v>3.9</v>
       </c>
       <c r="E11" t="s">
         <v>132</v>
@@ -6048,7 +6048,7 @@
         <v>110</v>
       </c>
       <c r="D12">
-        <v>12.67</v>
+        <v>12.7</v>
       </c>
       <c r="E12" t="s">
         <v>132</v>
@@ -6208,7 +6208,7 @@
         <v>115</v>
       </c>
       <c r="D17">
-        <v>5.34</v>
+        <v>5.3</v>
       </c>
       <c r="E17" t="s">
         <v>132</v>
@@ -6240,7 +6240,7 @@
         <v>116</v>
       </c>
       <c r="D18">
-        <v>15.74</v>
+        <v>15.7</v>
       </c>
       <c r="E18" t="s">
         <v>132</v>
@@ -6272,7 +6272,7 @@
         <v>117</v>
       </c>
       <c r="D19">
-        <v>5.15</v>
+        <v>5.1</v>
       </c>
       <c r="E19" t="s">
         <v>132</v>
@@ -6304,7 +6304,7 @@
         <v>118</v>
       </c>
       <c r="D20">
-        <v>15.84</v>
+        <v>15.8</v>
       </c>
       <c r="E20" t="s">
         <v>132</v>
@@ -6464,7 +6464,7 @@
         <v>123</v>
       </c>
       <c r="D25">
-        <v>1.63</v>
+        <v>1.6</v>
       </c>
       <c r="E25" t="s">
         <v>131</v>
@@ -6496,7 +6496,7 @@
         <v>124</v>
       </c>
       <c r="D26">
-        <v>5.73</v>
+        <v>5.7</v>
       </c>
       <c r="E26" t="s">
         <v>132</v>
@@ -6528,7 +6528,7 @@
         <v>125</v>
       </c>
       <c r="D27">
-        <v>1.14</v>
+        <v>1.1</v>
       </c>
       <c r="E27" t="s">
         <v>131</v>
@@ -6560,7 +6560,7 @@
         <v>126</v>
       </c>
       <c r="D28">
-        <v>5.63</v>
+        <v>5.6</v>
       </c>
       <c r="E28" t="s">
         <v>132</v>
@@ -6773,7 +6773,7 @@
         <v>100</v>
       </c>
       <c r="D2">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="E2" t="s">
         <v>131</v>
@@ -6805,7 +6805,7 @@
         <v>101</v>
       </c>
       <c r="D3">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="E3" t="s">
         <v>131</v>
@@ -7029,7 +7029,7 @@
         <v>108</v>
       </c>
       <c r="D10">
-        <v>6.39</v>
+        <v>6.4</v>
       </c>
       <c r="E10" t="s">
         <v>132</v>
@@ -7061,7 +7061,7 @@
         <v>109</v>
       </c>
       <c r="D11">
-        <v>1.66</v>
+        <v>1.7</v>
       </c>
       <c r="E11" t="s">
         <v>131</v>
@@ -7093,7 +7093,7 @@
         <v>110</v>
       </c>
       <c r="D12">
-        <v>6.39</v>
+        <v>6.4</v>
       </c>
       <c r="E12" t="s">
         <v>132</v>
@@ -7253,7 +7253,7 @@
         <v>115</v>
       </c>
       <c r="D17">
-        <v>2.51</v>
+        <v>2.5</v>
       </c>
       <c r="E17" t="s">
         <v>131</v>
@@ -7285,7 +7285,7 @@
         <v>116</v>
       </c>
       <c r="D18">
-        <v>8.25</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E18" t="s">
         <v>132</v>
@@ -7317,7 +7317,7 @@
         <v>117</v>
       </c>
       <c r="D19">
-        <v>2.18</v>
+        <v>2.2</v>
       </c>
       <c r="E19" t="s">
         <v>131</v>
@@ -7509,7 +7509,7 @@
         <v>123</v>
       </c>
       <c r="D25">
-        <v>0.54</v>
+        <v>0.5</v>
       </c>
       <c r="E25" t="s">
         <v>131</v>
@@ -7541,7 +7541,7 @@
         <v>124</v>
       </c>
       <c r="D26">
-        <v>2.11</v>
+        <v>2.1</v>
       </c>
       <c r="E26" t="s">
         <v>131</v>
@@ -7573,7 +7573,7 @@
         <v>125</v>
       </c>
       <c r="D27">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="E27" t="s">
         <v>131</v>
@@ -7605,7 +7605,7 @@
         <v>126</v>
       </c>
       <c r="D28">
-        <v>2.06</v>
+        <v>2.1</v>
       </c>
       <c r="E28" t="s">
         <v>131</v>
@@ -8042,7 +8042,7 @@
         <v>107</v>
       </c>
       <c r="D9">
-        <v>0.46</v>
+        <v>0.5</v>
       </c>
       <c r="E9" t="s">
         <v>131</v>
@@ -8074,7 +8074,7 @@
         <v>108</v>
       </c>
       <c r="D10">
-        <v>1.51</v>
+        <v>1.5</v>
       </c>
       <c r="E10" t="s">
         <v>131</v>
@@ -8106,7 +8106,7 @@
         <v>109</v>
       </c>
       <c r="D11">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="E11" t="s">
         <v>131</v>
@@ -8138,7 +8138,7 @@
         <v>110</v>
       </c>
       <c r="D12">
-        <v>1.56</v>
+        <v>1.6</v>
       </c>
       <c r="E12" t="s">
         <v>131</v>
@@ -8298,7 +8298,7 @@
         <v>115</v>
       </c>
       <c r="D17">
-        <v>0.76</v>
+        <v>0.8</v>
       </c>
       <c r="E17" t="s">
         <v>131</v>
@@ -8330,7 +8330,7 @@
         <v>116</v>
       </c>
       <c r="D18">
-        <v>2.36</v>
+        <v>2.4</v>
       </c>
       <c r="E18" t="s">
         <v>131</v>
@@ -8362,7 +8362,7 @@
         <v>117</v>
       </c>
       <c r="D19">
-        <v>0.54</v>
+        <v>0.5</v>
       </c>
       <c r="E19" t="s">
         <v>131</v>
@@ -8394,7 +8394,7 @@
         <v>118</v>
       </c>
       <c r="D20">
-        <v>2.36</v>
+        <v>2.4</v>
       </c>
       <c r="E20" t="s">
         <v>131</v>
@@ -9151,7 +9151,7 @@
         <v>109</v>
       </c>
       <c r="D11">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E11" t="s">
         <v>131</v>
@@ -9183,7 +9183,7 @@
         <v>110</v>
       </c>
       <c r="D12">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="E12" t="s">
         <v>131</v>
@@ -9343,7 +9343,7 @@
         <v>115</v>
       </c>
       <c r="D17">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E17" t="s">
         <v>131</v>
@@ -9375,7 +9375,7 @@
         <v>116</v>
       </c>
       <c r="D18">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="E18" t="s">
         <v>131</v>
@@ -9407,7 +9407,7 @@
         <v>117</v>
       </c>
       <c r="D19">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="E19" t="s">
         <v>131</v>
@@ -9439,7 +9439,7 @@
         <v>118</v>
       </c>
       <c r="D20">
-        <v>0.55</v>
+        <v>0.6</v>
       </c>
       <c r="E20" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
Added operative temperature test
</commit_message>
<xml_diff>
--- a/tests/testdata/tm52/TM52__TestJob1.xlsx
+++ b/tests/testdata/tm52/TM52__TestJob1.xlsx
@@ -30,15 +30,15 @@
     <t>JobNo</t>
   </si>
   <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>Author</t>
   </si>
   <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -75,45 +75,45 @@
     <t>/c/e</t>
   </si>
   <si>
+    <t>Project Information</t>
+  </si>
+  <si>
+    <t>Criterion % Definitions</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.15</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.2</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.3</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.4</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.5</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.6</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.7</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.8</t>
+  </si>
+  <si>
+    <t>20220223</t>
+  </si>
+  <si>
     <t>jovyan</t>
   </si>
   <si>
-    <t>Project Information</t>
-  </si>
-  <si>
-    <t>Criterion % Definitions</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.15</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.2</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.3</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.4</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.5</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.6</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.7</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.8</t>
-  </si>
-  <si>
-    <t>20220223</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -180,7 +180,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-02-23 16:02:16.314492</t>
+    <t>2022-02-23 18:10:45.877039</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -608,9 +608,9 @@
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="JobNo"/>
-    <tableColumn id="3" name="Author"/>
-    <tableColumn id="4" name="sheet_name"/>
-    <tableColumn id="5" name="Date"/>
+    <tableColumn id="3" name="sheet_name"/>
+    <tableColumn id="4" name="Date"/>
+    <tableColumn id="5" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1137,7 +1137,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>28</v>
@@ -1151,10 +1151,10 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>28</v>
@@ -1168,10 +1168,10 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
@@ -1185,10 +1185,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
@@ -1202,10 +1202,10 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
@@ -1219,10 +1219,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>
@@ -1236,10 +1236,10 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>28</v>
@@ -1253,10 +1253,10 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -1270,10 +1270,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>28</v>
@@ -1287,10 +1287,10 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
@@ -1304,7 +1304,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Added asserts to tests and added setup_class
</commit_message>
<xml_diff>
--- a/tests/testdata/tm52/TM52__TestJob1.xlsx
+++ b/tests/testdata/tm52/TM52__TestJob1.xlsx
@@ -30,15 +30,15 @@
     <t>Date</t>
   </si>
   <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
     <t>JobNo</t>
   </si>
   <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -72,48 +72,48 @@
     <t>10</t>
   </si>
   <si>
-    <t>20220223</t>
+    <t>20220224</t>
+  </si>
+  <si>
+    <t>jovyan</t>
+  </si>
+  <si>
+    <t>Project Information</t>
+  </si>
+  <si>
+    <t>Criterion % Definitions</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.15</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.2</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.3</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.4</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.5</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.6</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.7</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.8</t>
   </si>
   <si>
     <t>/c/e</t>
   </si>
   <si>
-    <t>Project Information</t>
-  </si>
-  <si>
-    <t>Criterion % Definitions</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.15</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.2</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.3</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.4</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.5</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.6</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.7</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.8</t>
-  </si>
-  <si>
-    <t>jovyan</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -180,7 +180,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-02-23 18:27:04.608414</t>
+    <t>2022-02-24 11:12:10.081416</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -608,9 +608,9 @@
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Date"/>
-    <tableColumn id="3" name="JobNo"/>
+    <tableColumn id="3" name="Author"/>
     <tableColumn id="4" name="sheet_name"/>
-    <tableColumn id="5" name="Author"/>
+    <tableColumn id="5" name="JobNo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>

<commit_message>
Updated tests. Pre-processing for ies tm52 report
</commit_message>
<xml_diff>
--- a/tests/testdata/tm52/TM52__TestJob1.xlsx
+++ b/tests/testdata/tm52/TM52__TestJob1.xlsx
@@ -27,18 +27,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="133">
   <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>JobNo</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>sheet_name</t>
   </si>
   <si>
-    <t>JobNo</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -72,12 +72,15 @@
     <t>10</t>
   </si>
   <si>
+    <t>jovyan</t>
+  </si>
+  <si>
+    <t>/c/e</t>
+  </si>
+  <si>
     <t>20220224</t>
   </si>
   <si>
-    <t>jovyan</t>
-  </si>
-  <si>
     <t>Project Information</t>
   </si>
   <si>
@@ -111,9 +114,6 @@
     <t>Results, Air Speed 0.8</t>
   </si>
   <si>
-    <t>/c/e</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -180,7 +180,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-02-24 11:12:10.081416</t>
+    <t>2022-02-24 13:15:49.867676</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -607,10 +607,10 @@
   <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="Date"/>
-    <tableColumn id="3" name="Author"/>
-    <tableColumn id="4" name="sheet_name"/>
-    <tableColumn id="5" name="JobNo"/>
+    <tableColumn id="2" name="Author"/>
+    <tableColumn id="3" name="JobNo"/>
+    <tableColumn id="4" name="Date"/>
+    <tableColumn id="5" name="sheet_name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1140,7 +1140,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1154,10 +1154,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1171,10 +1171,10 @@
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1188,10 +1188,10 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1205,10 +1205,10 @@
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1222,10 +1222,10 @@
         <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1239,10 +1239,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1256,10 +1256,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1273,10 +1273,10 @@
         <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1290,10 +1290,10 @@
         <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1307,7 +1307,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Created test notebook for docs
</commit_message>
<xml_diff>
--- a/tests/testdata/tm52/TM52__TestJob1.xlsx
+++ b/tests/testdata/tm52/TM52__TestJob1.xlsx
@@ -27,18 +27,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="133">
   <si>
+    <t>Author</t>
+  </si>
+  <si>
     <t>sheet_name</t>
   </si>
   <si>
+    <t>JobNo</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>JobNo</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -72,6 +72,9 @@
     <t>10</t>
   </si>
   <si>
+    <t>jovyan</t>
+  </si>
+  <si>
     <t>Project Information</t>
   </si>
   <si>
@@ -105,13 +108,10 @@
     <t>Results, Air Speed 0.8</t>
   </si>
   <si>
-    <t>20220224</t>
-  </si>
-  <si>
     <t>/c/e</t>
   </si>
   <si>
-    <t>jovyan</t>
+    <t>20220225</t>
   </si>
   <si>
     <t>index</t>
@@ -180,7 +180,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-02-24 17:21:32.315860</t>
+    <t>2022-02-25 14:06:11.166802</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -607,10 +607,10 @@
   <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="sheet_name"/>
-    <tableColumn id="3" name="Date"/>
+    <tableColumn id="2" name="Author"/>
+    <tableColumn id="3" name="sheet_name"/>
     <tableColumn id="4" name="JobNo"/>
-    <tableColumn id="5" name="Author"/>
+    <tableColumn id="5" name="Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1134,7 +1134,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>27</v>
@@ -1148,10 +1148,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>27</v>
@@ -1165,10 +1165,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>27</v>
@@ -1182,10 +1182,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>27</v>
@@ -1199,10 +1199,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>27</v>
@@ -1216,10 +1216,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>27</v>
@@ -1233,10 +1233,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>27</v>
@@ -1250,10 +1250,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>27</v>
@@ -1267,10 +1267,10 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>27</v>
@@ -1284,10 +1284,10 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>27</v>
@@ -1301,7 +1301,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>26</v>

</xml_diff>